<commit_message>
email receive automation done
</commit_message>
<xml_diff>
--- a/RPA/Order.xlsx
+++ b/RPA/Order.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Deloitte\Prototype\RPA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43C678EF-E50A-48BE-8E4A-C9AB63EC075A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FDA2FEA-8D5D-4D3D-9766-01EF117DFCD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
     <x:workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
@@ -31,13 +31,15 @@
     <x:t>text</x:t>
   </x:si>
   <x:si>
-    <x:t>kumarshresth2004@gmail.com</x:t>
+    <x:t>"Deepesh Gavali" &lt;deepzgavali143@gmail.com&gt;</x:t>
   </x:si>
   <x:si>
-    <x:t>Order Error</x:t>
+    <x:t>Order</x:t>
   </x:si>
   <x:si>
-    <x:t>Error processing order: [{'product': 'iPhone 15', 'requested': 3, 'available': 2}, {'product': 'Macbook Pro', 'requested': 2, 'available': 0}]</x:t>
+    <x:t xml:space="preserve">Hello
+I would like to order 2 MacBook and 1 iPhone
+</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -370,7 +372,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="C2:C3"/>
+  <x:dimension ref="C3"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0"/>
   </x:sheetViews>
@@ -386,14 +388,14 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <x:row r="2" spans="1:3">
       <x:c r="A2" s="0" t="s">
         <x:v>1</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="C2" s="0" t="s">
+      <x:c r="C2" s="1" t="s">
         <x:v>3</x:v>
       </x:c>
     </x:row>

</xml_diff>

<commit_message>
UiPath and Flask Integration
</commit_message>
<xml_diff>
--- a/RPA/Order.xlsx
+++ b/RPA/Order.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Deloitte\Prototype\RPA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FDA2FEA-8D5D-4D3D-9766-01EF117DFCD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06337D6D-A102-4AA5-BA92-6B9AA47FB840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <x:workbookView xWindow="0" yWindow="0" windowWidth="17280" windowHeight="9420" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,10 +40,10 @@
     <x:t>"Kumar Shresth" &lt;kshresth_be22@thapar.edu&gt;</x:t>
   </x:si>
   <x:si>
-    <x:t>Order</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">New order of IPhone 15
+    <x:t>Order50</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">iPhone,quantity:2
 </x:t>
   </x:si>
 </x:sst>
@@ -377,9 +377,11 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="C3"/>
+  <x:dimension ref="A1:C3"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" workbookViewId="0"/>
+    <x:sheetView tabSelected="1" workbookViewId="0">
+      <x:selection activeCell="C2" sqref="C2"/>
+    </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <x:cols>
@@ -388,7 +390,7 @@
     <x:col min="3" max="3" width="45.554688" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:3">
+    <x:row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -399,7 +401,7 @@
         <x:v>2</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:3">
+    <x:row r="2" spans="1:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A2" s="0" t="s">
         <x:v>3</x:v>
       </x:c>
@@ -410,7 +412,7 @@
         <x:v>5</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:3" ht="409.6" customHeight="1" x14ac:dyDescent="0.3">
+    <x:row r="3" spans="1:3" ht="409.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="C3" s="1"/>
     </x:row>
   </x:sheetData>

</xml_diff>